<commit_message>
add excel  template and feels
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/template.xlsx
+++ b/src/main/resources/templates/excel/template.xlsx
@@ -2,24 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\Projects\atb.su\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\java\Projects\atb.su\Inventory list\src\main\resources\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11400" windowHeight="5895" tabRatio="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11400" windowHeight="5895" tabRatio="312"/>
   </bookViews>
   <sheets>
     <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Унифицированная форма № ТОРГ-13</t>
   </si>
@@ -131,40 +131,31 @@
     <t>Получил</t>
   </si>
   <si>
-    <t>~{@DocNum}</t>
-  </si>
-  <si>
-    <t>~{@DocDate}</t>
-  </si>
-  <si>
-    <t>~@{DestinationDep}</t>
-  </si>
-  <si>
-    <t>~{@SourceDep}</t>
-  </si>
-  <si>
-    <t>~{@invNumberName}</t>
-  </si>
-  <si>
-    <t>~@{InvNumber}</t>
-  </si>
-  <si>
-    <t>~@{Total}</t>
-  </si>
-  <si>
-    <t>~@{SourceMol}</t>
-  </si>
-  <si>
-    <t>~@{DestinationMol}</t>
+    <t>ОО № 116</t>
+  </si>
+  <si>
+    <t>313005021</t>
+  </si>
+  <si>
+    <t>системный блок+клавиатура+мышь</t>
+  </si>
+  <si>
+    <t>Ивойлова Ирина Юмаровна</t>
+  </si>
+  <si>
+    <t>ОО № 50</t>
+  </si>
+  <si>
+    <t>Якимова Елена Сергеевна</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="000000000"/>
-    <numFmt numFmtId="175" formatCode="0&quot;шт&quot;"/>
+    <numFmt numFmtId="164" formatCode="000000000"/>
+    <numFmt numFmtId="165" formatCode="0&quot;шт&quot;"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -204,8 +195,10 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Arial Cyr"/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
@@ -215,11 +208,10 @@
       <charset val="204"/>
     </font>
     <font>
-      <u/>
-      <sz val="8"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -304,14 +296,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
         <color indexed="8"/>
       </bottom>
       <diagonal/>
@@ -320,10 +323,103 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="8"/>
       </right>
       <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
@@ -337,116 +433,16 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -484,32 +480,131 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -521,117 +616,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="10" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -690,7 +676,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -725,7 +711,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -916,13 +902,14 @@
   </sheetPr>
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30:L30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="19" width="10.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11" style="2" customWidth="1"/>
+    <col min="2" max="19" width="10.33203125" style="2" customWidth="1"/>
     <col min="20" max="21" width="10.6640625" customWidth="1"/>
     <col min="22" max="23" width="1.5" customWidth="1"/>
     <col min="24" max="24" width="38.33203125" bestFit="1" customWidth="1"/>
@@ -1000,24 +987,24 @@
       <c r="S3"/>
     </row>
     <row r="5" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
       <c r="S5"/>
     </row>
     <row r="9" spans="1:19" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1034,14 +1021,14 @@
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="50" t="s">
+      <c r="N9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50" t="s">
+      <c r="O9" s="21"/>
+      <c r="P9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="Q9" s="50"/>
+      <c r="Q9" s="21"/>
       <c r="R9" s="5"/>
       <c r="S9"/>
     </row>
@@ -1061,268 +1048,268 @@
       </c>
       <c r="L10"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="51"/>
-      <c r="P10" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q10" s="52"/>
+      <c r="N10" s="22">
+        <v>4</v>
+      </c>
+      <c r="O10" s="22"/>
+      <c r="P10" s="23">
+        <v>43143</v>
+      </c>
+      <c r="Q10" s="24"/>
       <c r="R10" s="4"/>
       <c r="S10"/>
     </row>
     <row r="11" spans="1:19" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="53"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="53"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
       <c r="S11"/>
     </row>
     <row r="13" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="46" t="s">
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
       <c r="R13" s="7"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:19" ht="49.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+    <row r="14" spans="1:19" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="48" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="49" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="48" t="s">
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48" t="s">
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
       <c r="R14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="S14" s="10"/>
     </row>
     <row r="15" spans="1:19" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40" t="s">
+      <c r="A15" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="31"/>
+      <c r="C15" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
       <c r="R15" s="11"/>
       <c r="S15" s="12"/>
     </row>
     <row r="17" spans="1:29" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="43" t="s">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="34" t="s">
+      <c r="J17" s="38"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
       <c r="S17"/>
     </row>
     <row r="18" spans="1:29" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18"/>
+    </row>
+    <row r="19" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="44" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18"/>
-    </row>
-    <row r="19" spans="1:29" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="13" t="s">
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="34" t="s">
+      <c r="J19" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34" t="s">
+      <c r="K19" s="36"/>
+      <c r="L19" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34" t="s">
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="34"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
       <c r="S19"/>
     </row>
-    <row r="20" spans="1:29" ht="13.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35">
+    <row r="20" spans="1:29" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="43">
         <v>1</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="14">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="17">
         <v>2</v>
       </c>
-      <c r="J20" s="37">
+      <c r="J20" s="45">
         <v>3</v>
       </c>
-      <c r="K20" s="37"/>
-      <c r="L20" s="38">
+      <c r="K20" s="45"/>
+      <c r="L20" s="46">
         <v>4</v>
       </c>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38">
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43">
         <v>5</v>
       </c>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
       <c r="S20"/>
     </row>
     <row r="21" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="15" t="s">
+      <c r="A21" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="33">
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="47">
         <v>1</v>
       </c>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
       <c r="S21"/>
     </row>
     <row r="22" spans="1:29" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
@@ -1337,17 +1324,15 @@
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
-      <c r="L22" s="17" t="s">
+      <c r="L22" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="60" t="s">
-        <v>42</v>
-      </c>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
       <c r="S22"/>
     </row>
     <row r="23" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1362,39 +1347,39 @@
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
-      <c r="L23" s="17" t="s">
+      <c r="L23" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
       <c r="S23"/>
-      <c r="Y23" s="20"/>
+      <c r="Y23" s="16"/>
     </row>
     <row r="24" spans="1:29" ht="15" x14ac:dyDescent="0.25">
-      <c r="Y24" s="20"/>
+      <c r="Y24" s="16"/>
     </row>
     <row r="25" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
       <c r="F25"/>
-      <c r="G25" s="61" t="s">
-        <v>43</v>
-      </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="18" t="s">
+      <c r="G25" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="14" t="s">
         <v>29</v>
       </c>
       <c r="N25"/>
@@ -1403,27 +1388,27 @@
       <c r="Q25"/>
       <c r="R25"/>
       <c r="S25"/>
-      <c r="Y25" s="20"/>
+      <c r="Y25" s="16"/>
     </row>
     <row r="26" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26"/>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="24"/>
+      <c r="C26" s="57"/>
       <c r="D26"/>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F26"/>
-      <c r="G26" s="24" t="s">
+      <c r="G26" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
       <c r="M26"/>
       <c r="N26"/>
       <c r="O26"/>
@@ -1436,65 +1421,65 @@
       <c r="A27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="21"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
       <c r="S27"/>
     </row>
     <row r="28" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28"/>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="55"/>
       <c r="S28"/>
     </row>
     <row r="29" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
       <c r="D29"/>
       <c r="E29" s="1"/>
       <c r="F29"/>
-      <c r="G29" s="61" t="s">
-        <v>44</v>
-      </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
+      <c r="G29" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
       <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
@@ -1504,21 +1489,21 @@
       <c r="S29"/>
     </row>
     <row r="30" spans="1:29" s="2" customFormat="1" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="E30" s="19" t="s">
+      <c r="C30" s="57"/>
+      <c r="E30" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="24" t="s">
+      <c r="G30" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="U31" s="2"/>
@@ -1554,12 +1539,52 @@
       <c r="AC33" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="A5:R5"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
+  <mergeCells count="59">
+    <mergeCell ref="B28:R28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="G30:L30"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="G29:L29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="B27:R27"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="L17:R17"/>
+    <mergeCell ref="L18:R18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="N15:Q15"/>
     <mergeCell ref="C11:R11"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="F13:M13"/>
@@ -1569,61 +1594,13 @@
     <mergeCell ref="F14:J14"/>
     <mergeCell ref="K14:M14"/>
     <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="I17:K18"/>
-    <mergeCell ref="L17:R17"/>
-    <mergeCell ref="A18:E19"/>
-    <mergeCell ref="F18:H19"/>
-    <mergeCell ref="L18:R18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="O19:R19"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="B27:R27"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="G25:L25"/>
-    <mergeCell ref="B28:R28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="G30:L30"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="G29:L29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="A5:R5"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="N10" r:id="rId1"/>
-    <hyperlink ref="P10" r:id="rId2"/>
-    <hyperlink ref="A15" r:id="rId3"/>
-    <hyperlink ref="F15" r:id="rId4"/>
-    <hyperlink ref="A21" r:id="rId5"/>
-    <hyperlink ref="F21" r:id="rId6"/>
-    <hyperlink ref="O22" r:id="rId7"/>
-    <hyperlink ref="G25" r:id="rId8"/>
-    <hyperlink ref="G29" r:id="rId9"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId10"/>
+  <pageSetup paperSize="9" scale="88" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>